<commit_message>
fix(nombres.xlsx): The order of the sheets was modified to ensure that the correct sheet is loaded
</commit_message>
<xml_diff>
--- a/datasets/nombres.xlsx
+++ b/datasets/nombres.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56a18304d3763240/Documentos/Work/Banco de Bogota/name_classifier/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BC8B79C-99F7-40A5-BFCA-BA5F87063C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1BC8B79C-99F7-40A5-BFCA-BA5F87063C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F43400F-F741-4F29-9E41-9C258CDEB936}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8D462FF7-391B-4D8C-98B3-CD085D025AEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8D462FF7-391B-4D8C-98B3-CD085D025AEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$A$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -746,6 +746,302 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8CA9A-6264-4484-A9DF-8794B4B91149}">
+  <dimension ref="A1:A56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EEA278-02B5-46F4-9506-AFA122CDB126}">
   <dimension ref="A1:A56"/>
   <sheetViews>
@@ -753,582 +1049,286 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8CA9A-6264-4484-A9DF-8794B4B91149}">
-  <dimension ref="A1:A56"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>